<commit_message>
feat: out excel add time
</commit_message>
<xml_diff>
--- a/storage/src/main/resources/excel/order.xlsx
+++ b/storage/src/main/resources/excel/order.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="24045" windowHeight="12375"/>
+    <workbookView windowWidth="27945" windowHeight="12375"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t>订单明细</t>
   </si>
@@ -59,12 +59,27 @@
     <t>组件总数量</t>
   </si>
   <si>
+    <t>已入库组件总数</t>
+  </si>
+  <si>
+    <t>已出库良品组件总数</t>
+  </si>
+  <si>
+    <t>剩余待出库数量</t>
+  </si>
+  <si>
+    <t>超出出库数量</t>
+  </si>
+  <si>
     <t>单价(元)</t>
   </si>
   <si>
     <t>合计(元)</t>
   </si>
   <si>
+    <t>时间范围</t>
+  </si>
+  <si>
     <t>{.code}</t>
   </si>
   <si>
@@ -92,10 +107,25 @@
     <t>{.partSumCount}</t>
   </si>
   <si>
+    <t>{.partSumCountCal}</t>
+  </si>
+  <si>
+    <t>{.outStroageGoodsSumCount}</t>
+  </si>
+  <si>
+    <t>{.partSumCountSubOutStroageGoodsSumCount}</t>
+  </si>
+  <si>
+    <t>{.overPartSumCount}</t>
+  </si>
+  <si>
     <t>{.price}</t>
   </si>
   <si>
     <t>{.sum}</t>
+  </si>
+  <si>
+    <t>{.time}</t>
   </si>
 </sst>
 </file>
@@ -471,9 +501,18 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="11">
     <border>
       <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right/>
       <top/>
       <bottom/>
@@ -618,7 +657,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -630,34 +669,34 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="4" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -742,7 +781,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -758,23 +797,29 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1098,172 +1143,232 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L11"/>
+  <dimension ref="A1:P11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="P8" sqref="P8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="13.5"/>
   <cols>
     <col min="1" max="5" width="40.625" style="3" customWidth="1"/>
     <col min="6" max="7" width="30.625" style="3" customWidth="1"/>
-    <col min="8" max="10" width="20.625" style="3" customWidth="1"/>
-    <col min="11" max="11" width="30.625" style="3" customWidth="1"/>
-    <col min="12" max="16384" width="8.725" style="3"/>
+    <col min="8" max="14" width="20.625" style="3" customWidth="1"/>
+    <col min="15" max="15" width="30.625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="45.625" style="3" customWidth="1"/>
+    <col min="17" max="16384" width="8.725" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" s="1" customFormat="1" ht="40" customHeight="1" spans="1:11">
+    <row r="1" s="1" customFormat="1" ht="40" customHeight="1" spans="1:16">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="B1" s="5"/>
+      <c r="C1" s="5"/>
+      <c r="D1" s="5"/>
+      <c r="E1" s="5"/>
+      <c r="F1" s="5"/>
+      <c r="G1" s="5"/>
+      <c r="H1" s="5"/>
+      <c r="I1" s="5"/>
+      <c r="J1" s="5"/>
+      <c r="K1" s="5"/>
+      <c r="L1" s="5"/>
+      <c r="M1" s="5"/>
+      <c r="N1" s="5"/>
+      <c r="O1" s="5"/>
+      <c r="P1" s="5"/>
     </row>
-    <row r="2" s="2" customFormat="1" ht="21" customHeight="1" spans="1:11">
-      <c r="A2" s="5" t="s">
+    <row r="2" s="2" customFormat="1" ht="21" customHeight="1" spans="1:16">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="6" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="6" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="G2" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="H2" s="6" t="s">
+      <c r="H2" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="6" t="s">
+      <c r="I2" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="6" t="s">
+      <c r="K2" s="7" t="s">
         <v>11</v>
       </c>
+      <c r="L2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="M2" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="N2" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="O2" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="P2" s="6" t="s">
+        <v>16</v>
+      </c>
     </row>
-    <row r="3" s="1" customFormat="1" ht="23" customHeight="1" spans="1:11">
-      <c r="A3" s="7" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="8" t="s">
-        <v>13</v>
-      </c>
-      <c r="C3" s="9" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="8" t="s">
-        <v>15</v>
-      </c>
-      <c r="E3" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="8" t="s">
+    <row r="3" s="1" customFormat="1" ht="23" customHeight="1" spans="1:16">
+      <c r="A3" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="H3" s="8" t="s">
+      <c r="C3" s="10" t="s">
         <v>19</v>
       </c>
-      <c r="I3" s="8" t="s">
+      <c r="D3" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="E3" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="K3" s="8" t="s">
+      <c r="F3" s="9" t="s">
         <v>22</v>
       </c>
+      <c r="G3" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="9" t="s">
+        <v>29</v>
+      </c>
+      <c r="N3" s="9" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="8" t="s">
+        <v>32</v>
+      </c>
     </row>
-    <row r="4" spans="3:12">
-      <c r="C4" s="10"/>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
-      <c r="F4" s="10"/>
-      <c r="G4" s="10"/>
-      <c r="H4" s="10"/>
-      <c r="I4" s="10"/>
-      <c r="J4" s="10"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="10"/>
+    <row r="4" spans="3:16">
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
+      <c r="G4" s="11"/>
+      <c r="H4" s="11"/>
+      <c r="I4" s="11"/>
+      <c r="J4" s="11"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11"/>
+      <c r="M4" s="11"/>
+      <c r="N4" s="11"/>
+      <c r="O4" s="11"/>
+      <c r="P4" s="11"/>
     </row>
-    <row r="5" spans="3:12">
-      <c r="C5" s="10"/>
-      <c r="D5" s="10"/>
-      <c r="E5" s="10"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="10"/>
-      <c r="H5" s="10"/>
-      <c r="I5" s="10"/>
-      <c r="J5" s="10"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="10"/>
+    <row r="5" spans="3:16">
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
+      <c r="G5" s="11"/>
+      <c r="H5" s="11"/>
+      <c r="I5" s="11"/>
+      <c r="J5" s="11"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11"/>
+      <c r="M5" s="11"/>
+      <c r="N5" s="11"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="11"/>
     </row>
-    <row r="6" spans="3:12">
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10"/>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
+    <row r="6" spans="3:16">
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
+      <c r="I6" s="11"/>
+      <c r="J6" s="11"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11"/>
+      <c r="M6" s="11"/>
+      <c r="N6" s="11"/>
+      <c r="O6" s="11"/>
+      <c r="P6" s="11"/>
     </row>
-    <row r="7" spans="3:12">
-      <c r="C7" s="10"/>
-      <c r="D7" s="10"/>
-      <c r="E7" s="10"/>
-      <c r="F7" s="10"/>
-      <c r="G7" s="10"/>
-      <c r="H7" s="10"/>
-      <c r="I7" s="10"/>
-      <c r="J7" s="10"/>
-      <c r="K7" s="10"/>
-      <c r="L7" s="10"/>
+    <row r="7" spans="3:16">
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
+      <c r="I7" s="11"/>
+      <c r="J7" s="11"/>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11"/>
+      <c r="M7" s="11"/>
+      <c r="N7" s="11"/>
+      <c r="O7" s="11"/>
+      <c r="P7" s="11"/>
     </row>
-    <row r="8" spans="3:12">
-      <c r="C8" s="10"/>
-      <c r="D8" s="10"/>
-      <c r="E8" s="10"/>
-      <c r="F8" s="10"/>
-      <c r="G8" s="10"/>
-      <c r="H8" s="10"/>
-      <c r="I8" s="10"/>
-      <c r="J8" s="10"/>
-      <c r="K8" s="10"/>
-      <c r="L8" s="10"/>
+    <row r="8" spans="3:16">
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
+      <c r="G8" s="11"/>
+      <c r="H8" s="11"/>
+      <c r="I8" s="11"/>
+      <c r="J8" s="11"/>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11"/>
+      <c r="M8" s="11"/>
+      <c r="N8" s="11"/>
+      <c r="O8" s="11"/>
+      <c r="P8" s="11"/>
     </row>
-    <row r="11" spans="10:10">
-      <c r="J11" s="11"/>
+    <row r="11" spans="10:14">
+      <c r="J11" s="13"/>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13"/>
+      <c r="M11" s="13"/>
+      <c r="N11" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A1:P1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
feat: version finish a lot of require in order page
</commit_message>
<xml_diff>
--- a/storage/src/main/resources/excel/order.xlsx
+++ b/storage/src/main/resources/excel/order.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="9405" activeTab="2"/>
+    <workbookView windowWidth="23040" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,7 +75,7 @@
     <t>交货时间</t>
   </si>
   <si>
-    <t>Z</t>
+    <t>单价</t>
   </si>
   <si>
     <t>合计</t>
@@ -239,10 +239,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="22">
     <font>
@@ -283,6 +283,106 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="13"/>
       <color theme="3"/>
@@ -292,84 +392,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -382,36 +412,6 @@
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -422,13 +422,175 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -440,169 +602,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -649,39 +649,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -693,6 +660,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -723,6 +699,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -737,150 +722,165 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1251,8 +1251,8 @@
   <sheetPr/>
   <dimension ref="A1:U11"/>
   <sheetViews>
-    <sheetView topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="S2" sqref="S$1:S$1048576"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="S6" sqref="S6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.72477064220183" defaultRowHeight="15.35"/>
@@ -1687,8 +1687,8 @@
   <sheetPr/>
   <dimension ref="A1:O3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="K5" sqref="K5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8256880733945" defaultRowHeight="15.35" outlineLevelRow="2"/>

</xml_diff>